<commit_message>
small changes, adding submission documents
</commit_message>
<xml_diff>
--- a/Submissions/Project Log.xlsx
+++ b/Submissions/Project Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
   <si>
     <t>Team 3 Documentation</t>
   </si>
@@ -167,6 +167,119 @@
   <si>
     <t>utilized Mat's models and textures and changed existing functions to reflect this</t>
   </si>
+  <si>
+    <t>researched terrain generation with noise and bilinear interpolation</t>
+  </si>
+  <si>
+    <t>examined dr mihail's terrain code</t>
+  </si>
+  <si>
+    <t>found and studied the diamond-square algorithm for terrain generation</t>
+  </si>
+  <si>
+    <t>began coding DS alg, ran into array issues</t>
+  </si>
+  <si>
+    <t>implemented LinkedList to store characters</t>
+  </si>
+  <si>
+    <t>minor fixes to initial camera angle</t>
+  </si>
+  <si>
+    <t>working on iterating through the list and switching characters with 'q'</t>
+  </si>
+  <si>
+    <t>periodically worked on the heightmap array, would hit a wall and research break</t>
+  </si>
+  <si>
+    <t>bashed head against wall with arrays</t>
+  </si>
+  <si>
+    <t>shifting the locations of code initializations to get linked list working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">md </t>
+  </si>
+  <si>
+    <t>finally found a way to get a useful array (map())</t>
+  </si>
+  <si>
+    <t>made progress on diamond square, got it working properly for 5x5. Larger arrays are probematic</t>
+  </si>
+  <si>
+    <t>Met up to discuss algorithm issues and progress</t>
+  </si>
+  <si>
+    <t>worked on presentation</t>
+  </si>
+  <si>
+    <t>Debugged and commented the heightMap generator. It populates properly (tested up to 129x129)</t>
+  </si>
+  <si>
+    <t>Worked on applying the heightmap to the floor geometry. Ran into geometry disappearing issues...</t>
+  </si>
+  <si>
+    <t>Worked on debugging geom.</t>
+  </si>
+  <si>
+    <t>replaced linked list with array again for simplicity</t>
+  </si>
+  <si>
+    <t>allowed swapping of characters with r without removing a turn</t>
+  </si>
+  <si>
+    <t>adding enemy models within an enemy array</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">changing enemy model colors in blender for practice: material preview mode, make sure it's attached to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>object</t>
+    </r>
+  </si>
+  <si>
+    <t>came up with a rough draft for the HUD</t>
+  </si>
+  <si>
+    <t>trying to implement enemy movement using a self-made sleep function</t>
+  </si>
+  <si>
+    <t>added "actor" attribute to attach the class to an obj</t>
+  </si>
+  <si>
+    <t>updated github project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished debugging floor geometry. Floor renders properly. </t>
+  </si>
+  <si>
+    <t>Added a metho to round all heightMap values to quarter numbers for polygonal appearance</t>
+  </si>
+  <si>
+    <t>Added a temp wireframe to the floor for visibility purposes. Will be removed later</t>
+  </si>
+  <si>
+    <t>began exploring ways to redraw our map grid</t>
+  </si>
+  <si>
+    <t>began exploring ways to dynamically apply correct verticle height to models</t>
+  </si>
+  <si>
+    <t>Began working on unpacking animations</t>
+  </si>
+  <si>
+    <t>Tabling animations in favor of improving terrain</t>
+  </si>
+  <si>
+    <t>es, md</t>
+  </si>
+  <si>
+    <t>Discussed project work load and current issues in the project</t>
+  </si>
 </sst>
 </file>
 
@@ -175,7 +288,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -189,6 +302,12 @@
       <b/>
       <sz val="12.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -235,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -270,19 +389,28 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -501,7 +629,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="58.71"/>
+    <col customWidth="1" min="3" max="3" width="107.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1116,7 +1244,7 @@
       <c r="Z20" s="10"/>
     </row>
     <row r="21">
-      <c r="A21" s="14">
+      <c r="A21" s="6">
         <v>43872.0</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1150,13 +1278,13 @@
       <c r="Z21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="14">
+      <c r="A22" s="6">
         <v>43873.0</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="7"/>
@@ -1186,7 +1314,7 @@
     <row r="23">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="7"/>
@@ -1216,7 +1344,7 @@
     <row r="24">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="7"/>
@@ -1244,13 +1372,13 @@
       <c r="Z24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="14">
+      <c r="A25" s="6">
         <v>43875.0</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="7"/>
@@ -1280,7 +1408,7 @@
     <row r="26">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="7"/>
@@ -1310,7 +1438,7 @@
     <row r="27">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="7"/>
@@ -1339,10 +1467,10 @@
     </row>
     <row r="28">
       <c r="A28" s="10"/>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="10"/>
@@ -1372,7 +1500,7 @@
     <row r="29">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="10"/>
@@ -1400,13 +1528,13 @@
       <c r="Z29" s="10"/>
     </row>
     <row r="30">
-      <c r="A30" s="17">
+      <c r="A30" s="9">
         <v>43877.0</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D30" s="10"/>
@@ -1436,7 +1564,7 @@
     <row r="31">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="10"/>
@@ -1466,7 +1594,7 @@
     <row r="32">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="10"/>
@@ -1496,7 +1624,7 @@
     <row r="33">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="10"/>
@@ -1524,11 +1652,11 @@
       <c r="Z33" s="10"/>
     </row>
     <row r="34">
-      <c r="A34" s="18"/>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="14"/>
+      <c r="B34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="7"/>
@@ -1558,7 +1686,7 @@
     <row r="35">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="7"/>
@@ -1586,9 +1714,9 @@
       <c r="Z35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="18"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="7"/>
@@ -1616,13 +1744,13 @@
       <c r="Z36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="14">
+      <c r="A37" s="6">
         <v>43878.0</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="7"/>
@@ -1652,7 +1780,7 @@
     <row r="38">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D38" s="7"/>
@@ -1682,7 +1810,7 @@
     <row r="39">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="7"/>
@@ -1709,6 +1837,1056 @@
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
     </row>
+    <row r="40">
+      <c r="A40" s="15">
+        <v>43879.0</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="15">
+        <v>43880.0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="14">
+        <v>43881.0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
+      <c r="Y44" s="7"/>
+      <c r="Z44" s="7"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="15">
+        <v>43882.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="10"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="15">
+        <v>43883.0</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="10"/>
+      <c r="W48" s="10"/>
+      <c r="X48" s="10"/>
+      <c r="Y48" s="10"/>
+      <c r="Z48" s="10"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="6">
+        <v>43884.0</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="10"/>
+      <c r="B50" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="10"/>
+      <c r="V50" s="10"/>
+      <c r="W50" s="10"/>
+      <c r="X50" s="10"/>
+      <c r="Y50" s="10"/>
+      <c r="Z50" s="10"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+      <c r="N51" s="10"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="10"/>
+      <c r="W51" s="10"/>
+      <c r="X51" s="10"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="10"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="16">
+        <v>43885.0</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="12"/>
+      <c r="U52" s="12"/>
+      <c r="V52" s="12"/>
+      <c r="W52" s="12"/>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="10"/>
+      <c r="B53" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="10"/>
+      <c r="V53" s="10"/>
+      <c r="W53" s="10"/>
+      <c r="X53" s="10"/>
+      <c r="Y53" s="10"/>
+      <c r="Z53" s="10"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="19">
+        <v>43887.0</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10"/>
+      <c r="U54" s="10"/>
+      <c r="V54" s="10"/>
+      <c r="W54" s="10"/>
+      <c r="X54" s="10"/>
+      <c r="Y54" s="10"/>
+      <c r="Z54" s="10"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="19">
+        <v>43888.0</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="10"/>
+      <c r="V55" s="10"/>
+      <c r="W55" s="10"/>
+      <c r="X55" s="10"/>
+      <c r="Y55" s="10"/>
+      <c r="Z55" s="10"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="19">
+        <v>43889.0</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10"/>
+      <c r="V56" s="10"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="10"/>
+      <c r="Y56" s="10"/>
+      <c r="Z56" s="10"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="20">
+        <v>43890.0</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="7"/>
+      <c r="V59" s="7"/>
+      <c r="W59" s="7"/>
+      <c r="X59" s="7"/>
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="7"/>
+      <c r="Y60" s="7"/>
+      <c r="Z60" s="7"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="20">
+        <v>43891.0</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="7"/>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+      <c r="Y62" s="7"/>
+      <c r="Z62" s="7"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="10"/>
+      <c r="B65" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
+      <c r="V65" s="10"/>
+      <c r="W65" s="10"/>
+      <c r="X65" s="10"/>
+      <c r="Y65" s="10"/>
+      <c r="Z65" s="10"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="10"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
+      <c r="V66" s="10"/>
+      <c r="W66" s="10"/>
+      <c r="X66" s="10"/>
+      <c r="Y66" s="10"/>
+      <c r="Z66" s="10"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
+      <c r="V67" s="10"/>
+      <c r="W67" s="10"/>
+      <c r="X67" s="10"/>
+      <c r="Y67" s="10"/>
+      <c r="Z67" s="10"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="10"/>
+      <c r="V68" s="10"/>
+      <c r="W68" s="10"/>
+      <c r="X68" s="10"/>
+      <c r="Y68" s="10"/>
+      <c r="Z68" s="10"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="10"/>
+      <c r="X69" s="10"/>
+      <c r="Y69" s="10"/>
+      <c r="Z69" s="10"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="19">
+        <v>43892.0</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="10"/>
+      <c r="V70" s="10"/>
+      <c r="W70" s="10"/>
+      <c r="X70" s="10"/>
+      <c r="Y70" s="10"/>
+      <c r="Z70" s="10"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+      <c r="O71" s="10"/>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10"/>
+      <c r="U71" s="10"/>
+      <c r="V71" s="10"/>
+      <c r="W71" s="10"/>
+      <c r="X71" s="10"/>
+      <c r="Y71" s="10"/>
+      <c r="Z71" s="10"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="12"/>
+      <c r="B72" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="12"/>
+      <c r="S72" s="12"/>
+      <c r="T72" s="12"/>
+      <c r="U72" s="12"/>
+      <c r="V72" s="12"/>
+      <c r="W72" s="12"/>
+      <c r="X72" s="12"/>
+      <c r="Y72" s="12"/>
+      <c r="Z72" s="12"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added submission docs and working on attacking
</commit_message>
<xml_diff>
--- a/Submissions/Project Log.xlsx
+++ b/Submissions/Project Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
   <si>
     <t>Team 3 Documentation</t>
   </si>
@@ -279,6 +279,33 @@
   </si>
   <si>
     <t>Discussed project work load and current issues in the project</t>
+  </si>
+  <si>
+    <t>wrote a bulk of the project proposal</t>
+  </si>
+  <si>
+    <t>began reseaarching ways to set height dynamically, starting with raycasters</t>
+  </si>
+  <si>
+    <t>added the Vanilla Random map type and added light noise generation</t>
+  </si>
+  <si>
+    <t>met to discuss titlescreen and map issues</t>
+  </si>
+  <si>
+    <t>implmented raycasters to dynamically set height</t>
+  </si>
+  <si>
+    <t>added some terrain object models and included the raycaster technique in loading them</t>
+  </si>
+  <si>
+    <t>fixed the map unit problem. models are now centered on squares</t>
+  </si>
+  <si>
+    <t>cleaned up some code and added random placement functionality to the game board</t>
+  </si>
+  <si>
+    <t>began implementation of attacking</t>
   </si>
 </sst>
 </file>
@@ -354,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -413,6 +440,7 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2887,6 +2915,298 @@
       <c r="Y72" s="12"/>
       <c r="Z72" s="12"/>
     </row>
+    <row r="73">
+      <c r="A73" s="22"/>
+      <c r="B73" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="22"/>
+      <c r="M73" s="22"/>
+      <c r="N73" s="22"/>
+      <c r="O73" s="22"/>
+      <c r="P73" s="22"/>
+      <c r="Q73" s="22"/>
+      <c r="R73" s="22"/>
+      <c r="S73" s="22"/>
+      <c r="T73" s="22"/>
+      <c r="U73" s="22"/>
+      <c r="V73" s="22"/>
+      <c r="W73" s="22"/>
+      <c r="X73" s="22"/>
+      <c r="Y73" s="22"/>
+      <c r="Z73" s="22"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="19">
+        <v>43895.0</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
+      <c r="V74" s="10"/>
+      <c r="W74" s="10"/>
+      <c r="X74" s="10"/>
+      <c r="Y74" s="10"/>
+      <c r="Z74" s="10"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="19">
+        <v>43896.0</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
+      <c r="U75" s="10"/>
+      <c r="V75" s="10"/>
+      <c r="W75" s="10"/>
+      <c r="X75" s="10"/>
+      <c r="Y75" s="10"/>
+      <c r="Z75" s="10"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="16">
+        <v>43899.0</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+      <c r="O76" s="12"/>
+      <c r="P76" s="12"/>
+      <c r="Q76" s="12"/>
+      <c r="R76" s="12"/>
+      <c r="S76" s="12"/>
+      <c r="T76" s="12"/>
+      <c r="U76" s="12"/>
+      <c r="V76" s="12"/>
+      <c r="W76" s="12"/>
+      <c r="X76" s="12"/>
+      <c r="Y76" s="12"/>
+      <c r="Z76" s="12"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="10"/>
+      <c r="B77" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+      <c r="O77" s="10"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10"/>
+      <c r="U77" s="10"/>
+      <c r="V77" s="10"/>
+      <c r="W77" s="10"/>
+      <c r="X77" s="10"/>
+      <c r="Y77" s="10"/>
+      <c r="Z77" s="10"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+      <c r="O78" s="10"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="10"/>
+      <c r="R78" s="10"/>
+      <c r="S78" s="10"/>
+      <c r="T78" s="10"/>
+      <c r="U78" s="10"/>
+      <c r="V78" s="10"/>
+      <c r="W78" s="10"/>
+      <c r="X78" s="10"/>
+      <c r="Y78" s="10"/>
+      <c r="Z78" s="10"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="10"/>
+      <c r="N79" s="10"/>
+      <c r="O79" s="10"/>
+      <c r="P79" s="10"/>
+      <c r="Q79" s="10"/>
+      <c r="R79" s="10"/>
+      <c r="S79" s="10"/>
+      <c r="T79" s="10"/>
+      <c r="U79" s="10"/>
+      <c r="V79" s="10"/>
+      <c r="W79" s="10"/>
+      <c r="X79" s="10"/>
+      <c r="Y79" s="10"/>
+      <c r="Z79" s="10"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="19">
+        <v>43900.0</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
+      <c r="N80" s="10"/>
+      <c r="O80" s="10"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="10"/>
+      <c r="R80" s="10"/>
+      <c r="S80" s="10"/>
+      <c r="T80" s="10"/>
+      <c r="U80" s="10"/>
+      <c r="V80" s="10"/>
+      <c r="W80" s="10"/>
+      <c r="X80" s="10"/>
+      <c r="Y80" s="10"/>
+      <c r="Z80" s="10"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="7"/>
+      <c r="B81" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>